<commit_message>
Added an exploratorative dose-response meta-analysis
A similar method to standardize the doses for ulotaront and rlamitaront with that of hte animal studies was used. The difference is that instead of log, i used Michaelis Menten taken into cosndieration both the Emax and E50. There are generally not enough studies for this (i.e., 3) and not good data for ralmitaront (while for ulotaront I could use Gallupi et al to estimate the concentrations for the daily doses). Thus, this may not be used.
</commit_message>
<xml_diff>
--- a/data/rob_secondary_2024.01.24.xlsx
+++ b/data/rob_secondary_2024.01.24.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sksiafis/Documents/GitHub/LSR3_taar1_H/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E355D4-F959-B447-9315-3825A09298E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF8F00D-6C5E-9846-91A7-62DE4C01C528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23460" yWindow="-16400" windowWidth="22220" windowHeight="15700" xr2:uid="{5B321493-8628-1E4C-935B-6CFC743B201E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="52">
   <si>
     <t>D1</t>
   </si>
@@ -660,7 +660,7 @@
   <dimension ref="A1:J88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D83" sqref="D83"/>
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -909,7 +909,9 @@
       <c r="H8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="4"/>
+      <c r="I8" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="J8" s="4" t="s">
         <v>5</v>
       </c>
@@ -939,7 +941,9 @@
       <c r="H9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="2"/>
+      <c r="I9" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="J9" s="2" t="s">
         <v>5</v>
       </c>
@@ -969,7 +973,9 @@
       <c r="H10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="4"/>
+      <c r="I10" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="J10" s="4" t="s">
         <v>5</v>
       </c>
@@ -999,7 +1005,9 @@
       <c r="H11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I11" s="2"/>
+      <c r="I11" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="J11" s="2" t="s">
         <v>5</v>
       </c>
@@ -1029,7 +1037,9 @@
       <c r="H12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="4"/>
+      <c r="I12" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="J12" s="2" t="s">
         <v>5</v>
       </c>
@@ -1059,7 +1069,9 @@
       <c r="H13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I13" s="2"/>
+      <c r="I13" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="J13" s="2" t="s">
         <v>5</v>
       </c>
@@ -1089,7 +1101,9 @@
       <c r="H14" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I14" s="4"/>
+      <c r="I14" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="J14" s="4" t="s">
         <v>5</v>
       </c>
@@ -1119,7 +1133,9 @@
       <c r="H15" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I15" s="2"/>
+      <c r="I15" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="J15" s="2" t="s">
         <v>5</v>
       </c>
@@ -1149,7 +1165,9 @@
       <c r="H16" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I16" s="4"/>
+      <c r="I16" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="J16" s="4" t="s">
         <v>5</v>
       </c>
@@ -3009,7 +3027,9 @@
       <c r="H78" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I78" s="2"/>
+      <c r="I78" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="J78" s="2" t="s">
         <v>5</v>
       </c>
@@ -3039,7 +3059,9 @@
       <c r="H79" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I79" s="4"/>
+      <c r="I79" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="J79" s="4" t="s">
         <v>5</v>
       </c>
@@ -3069,7 +3091,9 @@
       <c r="H80" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I80" s="2"/>
+      <c r="I80" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="J80" s="2" t="s">
         <v>5</v>
       </c>
@@ -3337,14 +3361,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="66b5d41f-65e9-4808-95b5-49073c9d5630">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f7f8f54e-e19b-4cd3-934a-81b57a2c13ba" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3565,21 +3587,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="66b5d41f-65e9-4808-95b5-49073c9d5630">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f7f8f54e-e19b-4cd3-934a-81b57a2c13ba" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4EB8B42-1E5E-46D3-BE50-95104077392D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F5AED06-1D9E-4A9F-85B0-2D70E5AF734B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="66b5d41f-65e9-4808-95b5-49073c9d5630"/>
-    <ds:schemaRef ds:uri="f7f8f54e-e19b-4cd3-934a-81b57a2c13ba"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3604,9 +3625,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F5AED06-1D9E-4A9F-85B0-2D70E5AF734B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4EB8B42-1E5E-46D3-BE50-95104077392D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="66b5d41f-65e9-4808-95b5-49073c9d5630"/>
+    <ds:schemaRef ds:uri="f7f8f54e-e19b-4cd3-934a-81b57a2c13ba"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>